<commit_message>
Adding Account, Deck, and Card classes. Also updating the Gantt chart.
</commit_message>
<xml_diff>
--- a/Online Poker Gantt Chart.xlsx
+++ b/Online Poker Gantt Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9c61462447f2ad11/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TrevM\Desktop\401ProjV2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A146058-9CD3-4650-BDA9-B3B420DF62F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F567ECFF-2EE0-41EF-A5E6-B1D8714B6F68}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>Online Poker Gantt Chart</t>
   </si>
@@ -33,27 +33,9 @@
     <t>CS 401-01 Project</t>
   </si>
   <si>
-    <t>Git Hub rep: https://github.com/Carlosv1232/dealerProj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Built the Server/Client </t>
-  </si>
-  <si>
-    <t>Player "Accounts' are created</t>
-  </si>
-  <si>
-    <t>Start building each server room</t>
-  </si>
-  <si>
-    <t>GUI</t>
-  </si>
-  <si>
     <t xml:space="preserve">Poker Tournament simulation </t>
   </si>
   <si>
-    <t xml:space="preserve">Finishing Touches: the poker tournament </t>
-  </si>
-  <si>
     <t>Finishing Touches: The project itself</t>
   </si>
   <si>
@@ -69,47 +51,7 @@
     <t>Summary of the Task</t>
   </si>
   <si>
-    <t xml:space="preserve">The beginning of building BOTH the client and server for the online poker. Make sure the connections are build and can have the data transfer, build the needed classes for 'each' player. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">sign-up, logins, and saving-up the information,, it would be added to the player class. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">setting up the hierarchy of each hand(for example, a flush would beat a pair.) And has to be randomly generated. and must be unique. </t>
-  </si>
-  <si>
-    <t>Start building the 'MAIN' system of the tournaments</t>
-  </si>
-  <si>
-    <t>Genesis N</t>
-  </si>
-  <si>
-    <t>Carlos V</t>
-  </si>
-  <si>
-    <t>Vanessa T</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This part is the most difficult b/c this is having players playing tournaments so we need the following: 1) have  connection in the server, 2) have a voting system, 3) the turn system(bet, fold, check), 4) the poker GUI. 
-*** need to start on the log-in GUI menu. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Focusing on the GUI part of the project. As in creating the menu, then provide the information to the user, and the balance(money) of the user. We test to see the functions are working, how the server rooms would look like, and the game chat would be.   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poker menu is done. We start working on the simulation. Work on the algorithms of betting and the system dictates the winner based by ranking. i.e. the leader is called 'The King' and whoever is it is the winner. </t>
-  </si>
-  <si>
     <t>Group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">we work on the finishing touches of the project to make sure everything is working. Then we work on the practice mode of the online poker tournament. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">We work on whatever is causing problems in the tasks that we picked to work on, fix any errors there are. If time allows, we try to finish the practice mode during this time, as well as the chat system. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Everything should be done by now and should be working. If we can we can add stuff like a prize rewards system for extra credit. </t>
   </si>
   <si>
     <r>
@@ -136,9 +78,6 @@
     </r>
   </si>
   <si>
-    <t>FINAL WEEK</t>
-  </si>
-  <si>
     <t xml:space="preserve">Starting Date </t>
   </si>
   <si>
@@ -146,6 +85,54 @@
   </si>
   <si>
     <t>Total days to work on task</t>
+  </si>
+  <si>
+    <t>Build Class Prototypes</t>
+  </si>
+  <si>
+    <t>Update Documentation</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Start testing/building network connectivity</t>
+  </si>
+  <si>
+    <t>Work on finishing GUI and classes</t>
+  </si>
+  <si>
+    <t>Further discuss additions/changes for class prototypes</t>
+  </si>
+  <si>
+    <t>Ensure the project is complete</t>
+  </si>
+  <si>
+    <t>Git Hub rep: https://github.com/jaybee707/PokerProj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update the files we received from the previous group. Any minor changes or updates we need to make to documentation, such as the gantt chart, will be added during this time. </t>
+  </si>
+  <si>
+    <t>We will create all the necessary classes with prototype methods by this time. This gives us a better understanding of what's expected from each class.</t>
+  </si>
+  <si>
+    <t>This is the time where we can look back at the prototypes we've created, and decide on whether or not we need to make additional changes.</t>
+  </si>
+  <si>
+    <t>This is the core of the game. We should preform basic network tests to ensure we can play the game with multiple users.</t>
+  </si>
+  <si>
+    <t>This task is just work to be done towards finishing the project. The bulk of our project should be completed during this time.</t>
+  </si>
+  <si>
+    <t>We should be able to run a basic simulation of our project at this point.</t>
+  </si>
+  <si>
+    <t>Any additional changes needed should be finished during this time.</t>
+  </si>
+  <si>
+    <t>The project should be completed and ready for final project presentations. If we still need extra time for anything, this is the week to do it.</t>
   </si>
 </sst>
 </file>
@@ -184,7 +171,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,6 +190,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -216,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -224,11 +217,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,71 +517,65 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$5:$A$13</c:f>
+              <c:f>Sheet1!$A$5:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>Built the Server/Client </c:v>
+                  <c:v>Update Documentation</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Player "Accounts' are created</c:v>
+                  <c:v>Build Class Prototypes</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Start building the 'MAIN' system of the tournaments</c:v>
+                  <c:v>Further discuss additions/changes for class prototypes</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Start building each server room</c:v>
+                  <c:v>Start testing/building network connectivity</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>GUI</c:v>
+                  <c:v>Work on finishing GUI and classes</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Poker Tournament simulation </c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Finishing Touches: the poker tournament </c:v>
+                  <c:v>Finishing Touches: The project itself</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Finishing Touches: The project itself</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>FINAL WEEK</c:v>
+                  <c:v>Ensure the project is complete</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$5:$D$13</c:f>
+              <c:f>Sheet1!$D$5:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>43885</c:v>
+                  <c:v>43927</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43894</c:v>
+                  <c:v>43927</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43902</c:v>
+                  <c:v>43934</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43910</c:v>
+                  <c:v>43934</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43921</c:v>
+                  <c:v>43934</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43929</c:v>
+                  <c:v>43948</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43937</c:v>
+                  <c:v>43948</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43945</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>43953</c:v>
+                  <c:v>43955</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -756,59 +751,56 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$5:$A$13</c:f>
+              <c:f>Sheet1!$A$5:$A$12</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>Built the Server/Client </c:v>
+                  <c:v>Update Documentation</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Player "Accounts' are created</c:v>
+                  <c:v>Build Class Prototypes</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Start building the 'MAIN' system of the tournaments</c:v>
+                  <c:v>Further discuss additions/changes for class prototypes</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Start building each server room</c:v>
+                  <c:v>Start testing/building network connectivity</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>GUI</c:v>
+                  <c:v>Work on finishing GUI and classes</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Poker Tournament simulation </c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Finishing Touches: the poker tournament </c:v>
+                  <c:v>Finishing Touches: The project itself</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Finishing Touches: The project itself</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>FINAL WEEK</c:v>
+                  <c:v>Ensure the project is complete</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$5:$F$13</c:f>
+              <c:f>Sheet1!$F$5:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>7</c:v>
@@ -818,9 +810,6 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1526,15 +1515,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>3448050</xdr:colOff>
+      <xdr:colOff>3409950</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>2686050</xdr:colOff>
+      <xdr:colOff>2647950</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1825,10 +1814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1843,256 +1832,241 @@
     <col min="9" max="9" width="26.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
+    <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>28</v>
+      <c r="A4" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="E4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>32</v>
-      </c>
       <c r="G4" s="9" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D5" s="2">
-        <v>43885</v>
+        <v>43927</v>
       </c>
       <c r="E5" s="2">
-        <v>43893</v>
-      </c>
-      <c r="F5" s="7">
-        <v>8</v>
+        <v>43931</v>
+      </c>
+      <c r="F5" s="6">
+        <v>5</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2">
-        <v>43894</v>
+        <v>43927</v>
       </c>
       <c r="E6" s="2">
-        <v>43901</v>
-      </c>
-      <c r="F6" s="7">
-        <v>7</v>
+        <v>43931</v>
+      </c>
+      <c r="F6" s="6">
+        <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D7" s="2">
-        <v>43902</v>
+        <v>43934</v>
       </c>
       <c r="E7" s="2">
-        <v>43909</v>
-      </c>
-      <c r="F7" s="7">
+        <v>43940</v>
+      </c>
+      <c r="F7" s="6">
         <v>7</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D8" s="2">
-        <v>43910</v>
+        <v>43934</v>
       </c>
       <c r="E8" s="2">
-        <v>43920</v>
-      </c>
-      <c r="F8" s="7">
-        <v>10</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>21</v>
+        <v>43947</v>
+      </c>
+      <c r="F8" s="6">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D9" s="2">
-        <v>43921</v>
+        <v>43934</v>
       </c>
       <c r="E9" s="2">
-        <v>43928</v>
-      </c>
-      <c r="F9" s="7">
-        <v>7</v>
+        <v>43947</v>
+      </c>
+      <c r="F9" s="6">
+        <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="2">
+        <v>43948</v>
+      </c>
+      <c r="E10" s="2">
+        <v>43954</v>
+      </c>
+      <c r="F10" s="6">
         <v>7</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="2">
-        <v>43929</v>
-      </c>
-      <c r="E10" s="2">
-        <v>43936</v>
-      </c>
-      <c r="F10" s="7">
-        <v>7</v>
-      </c>
       <c r="G10" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
       <c r="D11" s="2">
-        <v>43937</v>
+        <v>43948</v>
       </c>
       <c r="E11" s="2">
-        <v>43944</v>
-      </c>
-      <c r="F11" s="7">
+        <v>43954</v>
+      </c>
+      <c r="F11" s="6">
         <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D12" s="2">
-        <v>43945</v>
+        <v>43955</v>
       </c>
       <c r="E12" s="2">
-        <v>43952</v>
-      </c>
-      <c r="F12" s="7">
+        <v>43962</v>
+      </c>
+      <c r="F12" s="6">
         <v>7</v>
       </c>
       <c r="G12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="2">
-        <v>43953</v>
-      </c>
-      <c r="E13" s="2">
-        <v>43962</v>
-      </c>
-      <c r="F13" s="7">
-        <v>9</v>
-      </c>
-      <c r="G13" t="s">
-        <v>27</v>
-      </c>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="6"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="6"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
     </row>
@@ -2120,14 +2094,6 @@
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
     </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-    </row>
-    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>